<commit_message>
qwen catalog 20feb 11.04am
</commit_message>
<xml_diff>
--- a/listino/IMOLARTE NET PRICE WHOLESALE EXTRA CEE.xlsx
+++ b/listino/IMOLARTE NET PRICE WHOLESALE EXTRA CEE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9180" windowHeight="10350"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9180" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
@@ -3538,7 +3538,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3546,7 +3546,15 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -3641,7 +3649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3678,13 +3686,7 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3692,6 +3694,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4004,8 +4039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.1640625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4032,59 +4067,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>1165</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="17" t="s">
         <v>844</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>845</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="M2" s="18"/>
+      <c r="N2" s="23" t="s">
         <v>1168</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="O2" s="18"/>
+      <c r="P2" s="24" t="s">
         <v>846</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="25"/>
+      <c r="R2" s="15" t="s">
         <v>1166</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="10" t="s">
+      <c r="S2" s="15"/>
+      <c r="T2" s="16" t="s">
         <v>1167</v>
       </c>
       <c r="U2" s="10"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="12"/>
       <c r="E3" t="s">
         <v>6</v>
       </c>
@@ -4137,13 +4179,13 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>44.72</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -4202,13 +4244,13 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="1">
         <v>31.736000000000004</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="1">
@@ -4267,13 +4309,13 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>36.783999999999999</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="1">
@@ -4332,13 +4374,13 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="1">
         <v>64.2</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="1">
@@ -4397,13 +4439,13 @@
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="1">
         <v>75.016000000000005</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="1">
@@ -4462,13 +4504,13 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="1">
         <v>23.080000000000002</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="1">
@@ -4527,13 +4569,13 @@
       <c r="A10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="1">
         <v>69.968000000000004</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="1">
@@ -4592,13 +4634,13 @@
       <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="1">
         <v>26.688000000000002</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="1">
@@ -4657,13 +4699,13 @@
       <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="1">
         <v>30.295999999999999</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>73</v>
       </c>
       <c r="E12" s="1">
@@ -4722,13 +4764,13 @@
       <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>80</v>
       </c>
       <c r="C13" s="1">
         <v>35.344000000000001</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>81</v>
       </c>
       <c r="E13" s="1">
@@ -4787,13 +4829,13 @@
       <c r="A14" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="1">
         <v>38.231999999999999</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>89</v>
       </c>
       <c r="E14" s="1">
@@ -4852,13 +4894,13 @@
       <c r="A15" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>96</v>
       </c>
       <c r="C15" s="1">
         <v>42.56</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E15" s="1">
@@ -4917,13 +4959,13 @@
       <c r="A16" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>104</v>
       </c>
       <c r="C16" s="1">
         <v>59.144000000000005</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E16" s="1">
@@ -4982,13 +5024,13 @@
       <c r="A17" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>112</v>
       </c>
       <c r="C17" s="1">
         <v>71.408000000000001</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>113</v>
       </c>
       <c r="E17" s="1">
@@ -5047,13 +5089,13 @@
       <c r="A18" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>120</v>
       </c>
       <c r="C18" s="1">
         <v>36.783999999999999</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>121</v>
       </c>
       <c r="E18" s="1">
@@ -5112,13 +5154,13 @@
       <c r="A19" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>128</v>
       </c>
       <c r="C19" s="1">
         <v>34.624000000000002</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>129</v>
       </c>
       <c r="E19" s="1">
@@ -5177,13 +5219,13 @@
       <c r="A20" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>136</v>
       </c>
       <c r="C20" s="1">
         <v>15.144</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>137</v>
       </c>
       <c r="E20" s="1">
@@ -5242,13 +5284,13 @@
       <c r="A21" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>144</v>
       </c>
       <c r="C21" s="1">
         <v>17.312000000000001</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>145</v>
       </c>
       <c r="E21" s="1">
@@ -5307,13 +5349,13 @@
       <c r="A22" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>152</v>
       </c>
       <c r="C22" s="1">
         <v>21.64</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>153</v>
       </c>
       <c r="E22" s="1">
@@ -5372,13 +5414,13 @@
       <c r="A23" t="s">
         <v>159</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>160</v>
       </c>
       <c r="C23" s="1">
         <v>16.591999999999999</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>161</v>
       </c>
       <c r="E23" s="1">
@@ -5437,13 +5479,13 @@
       <c r="A24" t="s">
         <v>167</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>168</v>
       </c>
       <c r="C24" s="1">
         <v>15.144</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>169</v>
       </c>
       <c r="E24" s="1">
@@ -5502,13 +5544,13 @@
       <c r="A25" t="s">
         <v>175</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>176</v>
       </c>
       <c r="C25" s="1">
         <v>17.312000000000001</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>177</v>
       </c>
       <c r="E25" s="1">
@@ -5567,13 +5609,13 @@
       <c r="A26" t="s">
         <v>183</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>184</v>
       </c>
       <c r="C26" s="1">
         <v>23.8</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>185</v>
       </c>
       <c r="E26" s="1">
@@ -5632,13 +5674,13 @@
       <c r="A27" t="s">
         <v>191</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>192</v>
       </c>
       <c r="C27" s="1">
         <v>29.576000000000001</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>193</v>
       </c>
       <c r="E27" s="1">
@@ -5697,13 +5739,13 @@
       <c r="A28" t="s">
         <v>199</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>200</v>
       </c>
       <c r="C28" s="1">
         <v>15.872</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>201</v>
       </c>
       <c r="E28" s="1">
@@ -5762,13 +5804,13 @@
       <c r="A29" t="s">
         <v>207</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>208</v>
       </c>
       <c r="C29" s="1">
         <v>21.64</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>209</v>
       </c>
       <c r="E29" s="1">
@@ -5827,13 +5869,13 @@
       <c r="A30" t="s">
         <v>215</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>216</v>
       </c>
       <c r="C30" s="1">
         <v>23.8</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>217</v>
       </c>
       <c r="E30" s="1">
@@ -5892,13 +5934,13 @@
       <c r="A31" t="s">
         <v>223</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>224</v>
       </c>
       <c r="C31" s="1">
         <v>28.128</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>225</v>
       </c>
       <c r="E31" s="1">
@@ -5957,13 +5999,13 @@
       <c r="A32" t="s">
         <v>231</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>232</v>
       </c>
       <c r="C32" s="1">
         <v>21.64</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>233</v>
       </c>
       <c r="E32" s="1">
@@ -6022,13 +6064,13 @@
       <c r="A33" t="s">
         <v>239</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>240</v>
       </c>
       <c r="C33" s="1">
         <v>23.080000000000002</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>241</v>
       </c>
       <c r="E33" s="1">
@@ -6087,13 +6129,13 @@
       <c r="A34" t="s">
         <v>247</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>248</v>
       </c>
       <c r="C34" s="1">
         <v>28.856000000000002</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="12" t="s">
         <v>249</v>
       </c>
       <c r="E34" s="1">
@@ -6152,13 +6194,13 @@
       <c r="A35" t="s">
         <v>255</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>256</v>
       </c>
       <c r="C35" s="1">
         <v>23.8</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>257</v>
       </c>
       <c r="E35" s="1">
@@ -6217,13 +6259,13 @@
       <c r="A36" t="s">
         <v>263</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>264</v>
       </c>
       <c r="C36" s="1">
         <v>45.44</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>265</v>
       </c>
       <c r="E36" s="1">
@@ -6282,13 +6324,13 @@
       <c r="A37" t="s">
         <v>271</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>272</v>
       </c>
       <c r="C37" s="1">
         <v>16.591999999999999</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>273</v>
       </c>
       <c r="E37" s="1">
@@ -6347,13 +6389,13 @@
       <c r="A38" t="s">
         <v>279</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>280</v>
       </c>
       <c r="C38" s="1">
         <v>13.704000000000001</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="12" t="s">
         <v>281</v>
       </c>
       <c r="E38" s="1">
@@ -6412,13 +6454,13 @@
       <c r="A39" t="s">
         <v>287</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>288</v>
       </c>
       <c r="C39" s="1">
         <v>31.016000000000005</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>289</v>
       </c>
       <c r="E39" s="1">
@@ -6477,13 +6519,13 @@
       <c r="A40" t="s">
         <v>295</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>296</v>
       </c>
       <c r="C40" s="1">
         <v>49.768000000000001</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>297</v>
       </c>
       <c r="E40" s="1">
@@ -6542,13 +6584,13 @@
       <c r="A41" t="s">
         <v>303</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>304</v>
       </c>
       <c r="C41" s="1">
         <v>36.064</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>305</v>
       </c>
       <c r="E41" s="1">
@@ -6607,13 +6649,13 @@
       <c r="A42" t="s">
         <v>311</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>312</v>
       </c>
       <c r="C42" s="1">
         <v>30.295999999999999</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>313</v>
       </c>
       <c r="E42" s="1">
@@ -6672,13 +6714,13 @@
       <c r="A43" t="s">
         <v>319</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>320</v>
       </c>
       <c r="C43" s="1">
         <v>44</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12" t="s">
         <v>321</v>
       </c>
       <c r="E43" s="1">
@@ -6737,13 +6779,13 @@
       <c r="A44" t="s">
         <v>327</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>328</v>
       </c>
       <c r="C44" s="1">
         <v>41.84</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="12" t="s">
         <v>329</v>
       </c>
       <c r="E44" s="1">
@@ -6802,13 +6844,13 @@
       <c r="A45" t="s">
         <v>335</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>336</v>
       </c>
       <c r="C45" s="1">
         <v>54.816000000000003</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>337</v>
       </c>
       <c r="E45" s="1">
@@ -6867,13 +6909,13 @@
       <c r="A46" t="s">
         <v>343</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>344</v>
       </c>
       <c r="C46" s="1">
         <v>59.872000000000007</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="12" t="s">
         <v>345</v>
       </c>
       <c r="E46" s="1">
@@ -6932,13 +6974,13 @@
       <c r="A47" t="s">
         <v>351</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>352</v>
       </c>
       <c r="C47" s="1">
         <v>25.968000000000004</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="12" t="s">
         <v>353</v>
       </c>
       <c r="E47" s="1">
@@ -6997,13 +7039,13 @@
       <c r="A48" t="s">
         <v>359</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>360</v>
       </c>
       <c r="C48" s="1">
         <v>25.968000000000004</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="12" t="s">
         <v>361</v>
       </c>
       <c r="E48" s="1">
@@ -7062,13 +7104,13 @@
       <c r="A49" t="s">
         <v>367</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>368</v>
       </c>
       <c r="C49" s="1">
         <v>29.576000000000001</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>369</v>
       </c>
       <c r="E49" s="1">
@@ -7127,13 +7169,13 @@
       <c r="A50" t="s">
         <v>375</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>376</v>
       </c>
       <c r="C50" s="1">
         <v>36.783999999999999</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>377</v>
       </c>
       <c r="E50" s="1">
@@ -7192,13 +7234,13 @@
       <c r="A51" t="s">
         <v>383</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>384</v>
       </c>
       <c r="C51" s="1">
         <v>42.56</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>385</v>
       </c>
       <c r="E51" s="1">
@@ -7257,13 +7299,13 @@
       <c r="A52" t="s">
         <v>391</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="12" t="s">
         <v>392</v>
       </c>
       <c r="C52" s="1">
         <v>13.704000000000001</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="12" t="s">
         <v>393</v>
       </c>
       <c r="E52" s="1">
@@ -7322,13 +7364,13 @@
       <c r="A53" t="s">
         <v>399</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="12" t="s">
         <v>400</v>
       </c>
       <c r="C53" s="1">
         <v>18.752000000000002</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="12" t="s">
         <v>401</v>
       </c>
       <c r="E53" s="1">
@@ -7387,13 +7429,13 @@
       <c r="A54" t="s">
         <v>407</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="12" t="s">
         <v>408</v>
       </c>
       <c r="C54" s="1">
         <v>22.36</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D54" s="12" t="s">
         <v>409</v>
       </c>
       <c r="E54" s="1">
@@ -7452,13 +7494,13 @@
       <c r="A55" t="s">
         <v>415</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="12" t="s">
         <v>416</v>
       </c>
       <c r="C55" s="1">
         <v>24.528000000000002</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="12" t="s">
         <v>417</v>
       </c>
       <c r="E55" s="1">
@@ -7517,13 +7559,13 @@
       <c r="A56" t="s">
         <v>423</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="12" t="s">
         <v>424</v>
       </c>
       <c r="C56" s="1">
         <v>27.408000000000001</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" s="12" t="s">
         <v>425</v>
       </c>
       <c r="E56" s="1">
@@ -7582,13 +7624,13 @@
       <c r="A57" t="s">
         <v>431</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="12" t="s">
         <v>432</v>
       </c>
       <c r="C57" s="1">
         <v>34.624000000000002</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="12" t="s">
         <v>433</v>
       </c>
       <c r="E57" s="1">
@@ -7647,13 +7689,13 @@
       <c r="A58" t="s">
         <v>439</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="12" t="s">
         <v>440</v>
       </c>
       <c r="C58" s="1">
         <v>24.528000000000002</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="12" t="s">
         <v>441</v>
       </c>
       <c r="E58" s="1">
@@ -7712,13 +7754,13 @@
       <c r="A59" t="s">
         <v>447</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12" t="s">
         <v>448</v>
       </c>
       <c r="C59" s="1">
         <v>62.752000000000002</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>449</v>
       </c>
       <c r="E59" s="1">
@@ -7777,13 +7819,13 @@
       <c r="A60" t="s">
         <v>455</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="12" t="s">
         <v>456</v>
       </c>
       <c r="C60" s="1">
         <v>11.544</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D60" s="12" t="s">
         <v>457</v>
       </c>
       <c r="E60" s="1">
@@ -7842,13 +7884,13 @@
       <c r="A61" t="s">
         <v>463</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="12" t="s">
         <v>464</v>
       </c>
       <c r="C61" s="1">
         <v>12.984000000000002</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>465</v>
       </c>
       <c r="E61" s="1">
@@ -7907,13 +7949,13 @@
       <c r="A62" t="s">
         <v>471</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="12" t="s">
         <v>472</v>
       </c>
       <c r="C62" s="1">
         <v>13.704000000000001</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="12" t="s">
         <v>473</v>
       </c>
       <c r="E62" s="1">
@@ -7972,13 +8014,13 @@
       <c r="A63" t="s">
         <v>479</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="12" t="s">
         <v>480</v>
       </c>
       <c r="C63" s="1">
         <v>13.704000000000001</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="12" t="s">
         <v>481</v>
       </c>
       <c r="E63" s="1">
@@ -8037,13 +8079,13 @@
       <c r="A64" t="s">
         <v>487</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="12" t="s">
         <v>488</v>
       </c>
       <c r="C64" s="1">
         <v>15.872</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="12" t="s">
         <v>489</v>
       </c>
       <c r="E64" s="1">
@@ -8102,13 +8144,13 @@
       <c r="A65" t="s">
         <v>495</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="12" t="s">
         <v>496</v>
       </c>
       <c r="C65" s="1">
         <v>22.36</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="12" t="s">
         <v>497</v>
       </c>
       <c r="E65" s="1">
@@ -8167,13 +8209,13 @@
       <c r="A66" t="s">
         <v>503</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="12" t="s">
         <v>504</v>
       </c>
       <c r="C66" s="1">
         <v>13.704000000000001</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D66" s="12" t="s">
         <v>505</v>
       </c>
       <c r="E66" s="1">
@@ -8232,13 +8274,13 @@
       <c r="A67" t="s">
         <v>511</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="12" t="s">
         <v>512</v>
       </c>
       <c r="C67" s="1">
         <v>15.872</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="12" t="s">
         <v>513</v>
       </c>
       <c r="E67" s="1">
@@ -8297,13 +8339,13 @@
       <c r="A68" t="s">
         <v>519</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="12" t="s">
         <v>520</v>
       </c>
       <c r="C68" s="1">
         <v>19.472000000000001</v>
       </c>
-      <c r="D68" s="13" t="s">
+      <c r="D68" s="12" t="s">
         <v>521</v>
       </c>
       <c r="E68" s="1">
@@ -8362,13 +8404,13 @@
       <c r="A69" t="s">
         <v>527</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="12" t="s">
         <v>528</v>
       </c>
       <c r="C69" s="1">
         <v>20.200000000000003</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="12" t="s">
         <v>529</v>
       </c>
       <c r="E69" s="1">
@@ -8427,13 +8469,13 @@
       <c r="A70" t="s">
         <v>535</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="12" t="s">
         <v>536</v>
       </c>
       <c r="C70" s="1">
         <v>21.64</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="D70" s="12" t="s">
         <v>537</v>
       </c>
       <c r="E70" s="1">
@@ -8492,13 +8534,13 @@
       <c r="A71" t="s">
         <v>543</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="12" t="s">
         <v>544</v>
       </c>
       <c r="C71" s="1">
         <v>28.856000000000002</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="12" t="s">
         <v>545</v>
       </c>
       <c r="E71" s="1">
@@ -8557,13 +8599,13 @@
       <c r="A72" t="s">
         <v>551</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="12" t="s">
         <v>552</v>
       </c>
       <c r="C72" s="1">
         <v>23.080000000000002</v>
       </c>
-      <c r="D72" s="13" t="s">
+      <c r="D72" s="12" t="s">
         <v>553</v>
       </c>
       <c r="E72" s="1">
@@ -8622,13 +8664,13 @@
       <c r="A73" t="s">
         <v>559</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="12" t="s">
         <v>560</v>
       </c>
       <c r="C73" s="1">
         <v>148.59200000000001</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="12" t="s">
         <v>561</v>
       </c>
       <c r="E73" s="1">
@@ -8687,13 +8729,13 @@
       <c r="A74" t="s">
         <v>567</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="12" t="s">
         <v>568</v>
       </c>
       <c r="C74" s="1">
         <v>132</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="D74" s="12" t="s">
         <v>569</v>
       </c>
       <c r="E74" s="1">
@@ -8752,13 +8794,13 @@
       <c r="A75" t="s">
         <v>575</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="12" t="s">
         <v>576</v>
       </c>
       <c r="C75" s="1">
         <v>25.968000000000004</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="12" t="s">
         <v>577</v>
       </c>
       <c r="E75" s="1">
@@ -8817,13 +8859,13 @@
       <c r="A76" t="s">
         <v>583</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="12" t="s">
         <v>584</v>
       </c>
       <c r="C76" s="1">
         <v>28.856000000000002</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="D76" s="12" t="s">
         <v>585</v>
       </c>
       <c r="E76" s="1">
@@ -8882,13 +8924,13 @@
       <c r="A77" t="s">
         <v>591</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B77" s="12" t="s">
         <v>592</v>
       </c>
       <c r="C77" s="1">
         <v>30.295999999999999</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="12" t="s">
         <v>593</v>
       </c>
       <c r="E77" s="1">
@@ -8947,13 +8989,13 @@
       <c r="A78" t="s">
         <v>599</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="12" t="s">
         <v>600</v>
       </c>
       <c r="C78" s="1">
         <v>27.408000000000001</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="12" t="s">
         <v>601</v>
       </c>
       <c r="E78" s="1">
@@ -9012,13 +9054,13 @@
       <c r="A79" t="s">
         <v>607</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B79" s="12" t="s">
         <v>608</v>
       </c>
       <c r="C79" s="1">
         <v>21.64</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="12" t="s">
         <v>609</v>
       </c>
       <c r="E79" s="1">
@@ -9077,13 +9119,13 @@
       <c r="A80" t="s">
         <v>615</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="12" t="s">
         <v>616</v>
       </c>
       <c r="C80" s="1">
         <v>21.64</v>
       </c>
-      <c r="D80" s="13" t="s">
+      <c r="D80" s="12" t="s">
         <v>617</v>
       </c>
       <c r="E80" s="1">
@@ -9142,13 +9184,13 @@
       <c r="A81" t="s">
         <v>623</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="12" t="s">
         <v>624</v>
       </c>
       <c r="C81" s="1">
         <v>15.872</v>
       </c>
-      <c r="D81" s="13" t="s">
+      <c r="D81" s="12" t="s">
         <v>625</v>
       </c>
       <c r="E81" s="1">
@@ -9207,13 +9249,13 @@
       <c r="A82" t="s">
         <v>631</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="12" t="s">
         <v>632</v>
       </c>
       <c r="C82" s="1">
         <v>24.528000000000002</v>
       </c>
-      <c r="D82" s="13" t="s">
+      <c r="D82" s="12" t="s">
         <v>633</v>
       </c>
       <c r="E82" s="1">
@@ -9272,13 +9314,13 @@
       <c r="A83" t="s">
         <v>639</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="12" t="s">
         <v>640</v>
       </c>
       <c r="C83" s="1">
         <v>36.064</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="12" t="s">
         <v>641</v>
       </c>
       <c r="E83" s="1">
@@ -9337,13 +9379,13 @@
       <c r="A84" t="s">
         <v>647</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B84" s="12" t="s">
         <v>648</v>
       </c>
       <c r="C84" s="1">
         <v>38.951999999999998</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D84" s="12" t="s">
         <v>649</v>
       </c>
       <c r="E84" s="1">
@@ -9402,13 +9444,13 @@
       <c r="A85" t="s">
         <v>655</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="12" t="s">
         <v>656</v>
       </c>
       <c r="C85" s="1">
         <v>19.472000000000001</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="12" t="s">
         <v>657</v>
       </c>
       <c r="E85" s="1">
@@ -9467,13 +9509,13 @@
       <c r="A86" t="s">
         <v>663</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B86" s="12" t="s">
         <v>664</v>
       </c>
       <c r="C86" s="1">
         <v>20.92</v>
       </c>
-      <c r="D86" s="13" t="s">
+      <c r="D86" s="12" t="s">
         <v>665</v>
       </c>
       <c r="E86" s="1">
@@ -9532,13 +9574,13 @@
       <c r="A87" t="s">
         <v>671</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="12" t="s">
         <v>672</v>
       </c>
       <c r="C87" s="1">
         <v>26.688000000000002</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D87" s="12" t="s">
         <v>673</v>
       </c>
       <c r="E87" s="1">
@@ -9597,13 +9639,13 @@
       <c r="A88" t="s">
         <v>679</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B88" s="12" t="s">
         <v>680</v>
       </c>
       <c r="C88" s="1">
         <v>28.128</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D88" s="12" t="s">
         <v>681</v>
       </c>
       <c r="E88" s="1">
@@ -9662,13 +9704,13 @@
       <c r="A89" t="s">
         <v>687</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="12" t="s">
         <v>688</v>
       </c>
       <c r="C89" s="1">
         <v>27.408000000000001</v>
       </c>
-      <c r="D89" s="13" t="s">
+      <c r="D89" s="12" t="s">
         <v>689</v>
       </c>
       <c r="E89" s="1">
@@ -9727,13 +9769,13 @@
       <c r="A90" t="s">
         <v>695</v>
       </c>
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="12" t="s">
         <v>696</v>
       </c>
       <c r="C90" s="1">
         <v>26.688000000000002</v>
       </c>
-      <c r="D90" s="13" t="s">
+      <c r="D90" s="12" t="s">
         <v>697</v>
       </c>
       <c r="E90" s="1">
@@ -9792,13 +9834,13 @@
       <c r="A91" t="s">
         <v>703</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="B91" s="12" t="s">
         <v>704</v>
       </c>
       <c r="C91" s="1">
         <v>25.968000000000004</v>
       </c>
-      <c r="D91" s="13" t="s">
+      <c r="D91" s="12" t="s">
         <v>705</v>
       </c>
       <c r="E91" s="1">
@@ -9857,13 +9899,13 @@
       <c r="A92" t="s">
         <v>711</v>
       </c>
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="12" t="s">
         <v>712</v>
       </c>
       <c r="C92" s="1">
         <v>49.768000000000001</v>
       </c>
-      <c r="D92" s="13" t="s">
+      <c r="D92" s="12" t="s">
         <v>713</v>
       </c>
       <c r="E92" s="1">
@@ -9922,13 +9964,13 @@
       <c r="A93" t="s">
         <v>719</v>
       </c>
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="12" t="s">
         <v>720</v>
       </c>
       <c r="C93" s="1">
         <v>58.424000000000007</v>
       </c>
-      <c r="D93" s="13" t="s">
+      <c r="D93" s="12" t="s">
         <v>721</v>
       </c>
       <c r="E93" s="1">
@@ -9987,13 +10029,13 @@
       <c r="A94" t="s">
         <v>727</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B94" s="12" t="s">
         <v>728</v>
       </c>
       <c r="C94" s="1">
         <v>58.424000000000007</v>
       </c>
-      <c r="D94" s="13" t="s">
+      <c r="D94" s="12" t="s">
         <v>729</v>
       </c>
       <c r="E94" s="1">
@@ -10052,13 +10094,13 @@
       <c r="A95" t="s">
         <v>735</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="12" t="s">
         <v>736</v>
       </c>
       <c r="C95" s="1">
         <v>69.248000000000005</v>
       </c>
-      <c r="D95" s="13" t="s">
+      <c r="D95" s="12" t="s">
         <v>737</v>
       </c>
       <c r="E95" s="1">
@@ -10117,13 +10159,13 @@
       <c r="A96" t="s">
         <v>1149</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="12" t="s">
         <v>743</v>
       </c>
       <c r="C96" s="1">
         <v>29.576000000000001</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D96" s="12" t="s">
         <v>744</v>
       </c>
       <c r="E96" s="1">
@@ -10182,13 +10224,13 @@
       <c r="A97" t="s">
         <v>1151</v>
       </c>
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="12" t="s">
         <v>750</v>
       </c>
       <c r="C97" s="1">
         <v>34.624000000000002</v>
       </c>
-      <c r="D97" s="13" t="s">
+      <c r="D97" s="12" t="s">
         <v>751</v>
       </c>
       <c r="E97" s="1">
@@ -10247,13 +10289,13 @@
       <c r="A98" t="s">
         <v>1153</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="12" t="s">
         <v>757</v>
       </c>
       <c r="C98" s="1">
         <v>57.704000000000001</v>
       </c>
-      <c r="D98" s="13" t="s">
+      <c r="D98" s="12" t="s">
         <v>758</v>
       </c>
       <c r="E98" s="1">
@@ -10312,13 +10354,13 @@
       <c r="A99" t="s">
         <v>764</v>
       </c>
-      <c r="B99" s="13" t="s">
+      <c r="B99" s="12" t="s">
         <v>765</v>
       </c>
       <c r="C99" s="1">
         <v>23.080000000000002</v>
       </c>
-      <c r="D99" s="13" t="s">
+      <c r="D99" s="12" t="s">
         <v>766</v>
       </c>
       <c r="E99" s="1">
@@ -10377,13 +10419,13 @@
       <c r="A100" t="s">
         <v>772</v>
       </c>
-      <c r="B100" s="13" t="s">
+      <c r="B100" s="12" t="s">
         <v>773</v>
       </c>
       <c r="C100" s="1">
         <v>33.183999999999997</v>
       </c>
-      <c r="D100" s="13" t="s">
+      <c r="D100" s="12" t="s">
         <v>774</v>
       </c>
       <c r="E100" s="1">
@@ -10442,13 +10484,13 @@
       <c r="A101" t="s">
         <v>780</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="12" t="s">
         <v>781</v>
       </c>
       <c r="C101" s="1">
         <v>16.591999999999999</v>
       </c>
-      <c r="D101" s="13" t="s">
+      <c r="D101" s="12" t="s">
         <v>782</v>
       </c>
       <c r="E101" s="1">
@@ -10507,13 +10549,13 @@
       <c r="A102" t="s">
         <v>788</v>
       </c>
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="12" t="s">
         <v>789</v>
       </c>
       <c r="C102" s="1">
         <v>122.62400000000001</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D102" s="12" t="s">
         <v>790</v>
       </c>
       <c r="E102" s="1">
@@ -10572,13 +10614,13 @@
       <c r="A103" t="s">
         <v>796</v>
       </c>
-      <c r="B103" s="13" t="s">
+      <c r="B103" s="12" t="s">
         <v>797</v>
       </c>
       <c r="C103" s="1">
         <v>41.84</v>
       </c>
-      <c r="D103" s="13" t="s">
+      <c r="D103" s="12" t="s">
         <v>798</v>
       </c>
       <c r="E103" s="1">
@@ -10637,13 +10679,13 @@
       <c r="A104" t="s">
         <v>804</v>
       </c>
-      <c r="B104" s="13" t="s">
+      <c r="B104" s="12" t="s">
         <v>805</v>
       </c>
       <c r="C104" s="1">
         <v>45.44</v>
       </c>
-      <c r="D104" s="13" t="s">
+      <c r="D104" s="12" t="s">
         <v>806</v>
       </c>
       <c r="E104" s="1">
@@ -10702,13 +10744,13 @@
       <c r="A105" t="s">
         <v>812</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B105" s="12" t="s">
         <v>813</v>
       </c>
       <c r="C105" s="1">
         <v>52.655999999999999</v>
       </c>
-      <c r="D105" s="13" t="s">
+      <c r="D105" s="12" t="s">
         <v>814</v>
       </c>
       <c r="E105" s="1">
@@ -10767,13 +10809,13 @@
       <c r="A106" t="s">
         <v>820</v>
       </c>
-      <c r="B106" s="13" t="s">
+      <c r="B106" s="12" t="s">
         <v>821</v>
       </c>
       <c r="C106" s="1">
         <v>132</v>
       </c>
-      <c r="D106" s="13" t="s">
+      <c r="D106" s="12" t="s">
         <v>822</v>
       </c>
       <c r="E106" s="1">
@@ -10832,13 +10874,13 @@
       <c r="A107" t="s">
         <v>828</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="12" t="s">
         <v>829</v>
       </c>
       <c r="C107" s="1">
         <v>165.184</v>
       </c>
-      <c r="D107" s="13" t="s">
+      <c r="D107" s="12" t="s">
         <v>830</v>
       </c>
       <c r="E107" s="1">
@@ -10897,13 +10939,13 @@
       <c r="A108" t="s">
         <v>836</v>
       </c>
-      <c r="B108" s="13" t="s">
+      <c r="B108" s="12" t="s">
         <v>837</v>
       </c>
       <c r="C108" s="1">
         <v>197.64000000000001</v>
       </c>
-      <c r="D108" s="13" t="s">
+      <c r="D108" s="12" t="s">
         <v>838</v>
       </c>
       <c r="E108" s="1">
@@ -10963,5 +11005,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>